<commit_message>
Adding fridge, ice drill, asteroid config.
</commit_message>
<xml_diff>
--- a/Tools/RealISRU.xlsx
+++ b/Tools/RealISRU.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="196">
   <si>
     <t>Process</t>
   </si>
@@ -153,6 +153,30 @@
   </si>
   <si>
     <t>Kerosene</t>
+  </si>
+  <si>
+    <t>Liquefy Oxygen</t>
+  </si>
+  <si>
+    <t>lqdOxygen</t>
+  </si>
+  <si>
+    <t>Liquefy Hydrogen</t>
+  </si>
+  <si>
+    <t>lqdHydrogen</t>
+  </si>
+  <si>
+    <t>Liquefy Ammonia</t>
+  </si>
+  <si>
+    <t>lqdAmmonia</t>
+  </si>
+  <si>
+    <t>Liquefy Methane</t>
+  </si>
+  <si>
+    <t>lqdMethane</t>
   </si>
   <si>
     <t>Resource Name</t>
@@ -881,8 +905,12 @@
   </sheetPr>
   <dimension ref="1:50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1690,7 +1718,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="1" t="n">
@@ -2441,7 +2469,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="7" t="s">
         <v>41</v>
       </c>
       <c r="E13" s="1" t="n">
@@ -2571,7 +2599,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="7" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="1" t="n">
@@ -2701,17 +2729,32 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G15" s="2" t="e">
+      <c r="A15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="n">
         <f aca="false">VLOOKUP(H15,Resources!$A$2:$F$799,5,0)/I15</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J15" s="2" t="e">
+        <v>0.0881305081567598</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2" t="n">
         <f aca="false">VLOOKUP(H15,Resources!$A$2:$F$799,4,0)*I15*G15</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K15" s="2" t="e">
+        <v>1.41E-006</v>
+      </c>
+      <c r="K15" s="2" t="n">
         <f aca="false">J15/VLOOKUP(H15,Resources!$A$2:$F$799,2,0)</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="N15" s="2" t="e">
         <f aca="false">VLOOKUP(L15,Resources!$A$2:$F$799,4,0)*M15*$G15</f>
@@ -2729,13 +2772,19 @@
         <f aca="false">R15/VLOOKUP(P15,Resources!$A$2:$F$799,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="V15" s="2" t="e">
+      <c r="T15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V15" s="2" t="n">
         <f aca="false">VLOOKUP(T15,Resources!$A$2:$F$799,4,0)*U15*$G15*$F15</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W15" s="2" t="e">
+        <v>2.82007050440653E-006</v>
+      </c>
+      <c r="W15" s="2" t="n">
         <f aca="false">V15/VLOOKUP(T15,Resources!$A$2:$F$799,2,0)</f>
-        <v>#N/A</v>
+        <v>0.00247157800561483</v>
       </c>
       <c r="Z15" s="2" t="e">
         <f aca="false">VLOOKUP(X15,Resources!$A$2:$F$799,4,0)*Y15*$G15*$F15</f>
@@ -2761,23 +2810,58 @@
         <f aca="false">AH15/VLOOKUP(AF15,Resources!$A$2:$F$799,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="AJ15" s="3" t="str">
+      <c r="AJ15" s="8" t="str">
         <f aca="false">Config!A15</f>
-        <v/>
+        <v>    MODULE
+    {
+        name = ModuleResourceConverter
+        ConverterName = Liquefy Oxygen
+        StartActionName = Start Liquefy Oxygen
+        StopActionName = Stop Liquefy Oxygen
+        AutoShutdown = false
+        GeneratesHeat = true
+        UseSpecialistBonus = false
+        INPUT_RESOURCE
+        {
+            ResourceName = Oxygen
+            Ratio = 1
+        }
+        OUTPUT_RESOURCE
+        {
+            ResourceName = lqdOxygen
+            Ratio = 0.00247157800561483
+            DumpExcess = false
+        }
+    }</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G16" s="2" t="e">
+      <c r="A16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="n">
         <f aca="false">VLOOKUP(H16,Resources!$A$2:$F$799,5,0)/I16</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J16" s="2" t="e">
+        <v>0.0891953566822106</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2" t="n">
         <f aca="false">VLOOKUP(H16,Resources!$A$2:$F$799,4,0)*I16*G16</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K16" s="2" t="e">
+        <v>8.99E-008</v>
+      </c>
+      <c r="K16" s="2" t="n">
         <f aca="false">J16/VLOOKUP(H16,Resources!$A$2:$F$799,2,0)</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="N16" s="2" t="e">
         <f aca="false">VLOOKUP(L16,Resources!$A$2:$F$799,4,0)*M16*$G16</f>
@@ -2795,13 +2879,19 @@
         <f aca="false">R16/VLOOKUP(P16,Resources!$A$2:$F$799,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="V16" s="2" t="e">
+      <c r="T16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V16" s="2" t="n">
         <f aca="false">VLOOKUP(T16,Resources!$A$2:$F$799,4,0)*U16*$G16*$F16</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W16" s="2" t="e">
+        <v>1.79807135628535E-007</v>
+      </c>
+      <c r="W16" s="2" t="n">
         <f aca="false">V16/VLOOKUP(T16,Resources!$A$2:$F$799,2,0)</f>
-        <v>#N/A</v>
+        <v>0.00253785653674714</v>
       </c>
       <c r="Z16" s="2" t="e">
         <f aca="false">VLOOKUP(X16,Resources!$A$2:$F$799,4,0)*Y16*$G16*$F16</f>
@@ -2827,23 +2917,58 @@
         <f aca="false">AH16/VLOOKUP(AF16,Resources!$A$2:$F$799,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="AJ16" s="3" t="str">
+      <c r="AJ16" s="8" t="str">
         <f aca="false">Config!A16</f>
-        <v/>
+        <v>    MODULE
+    {
+        name = ModuleResourceConverter
+        ConverterName = Liquefy Hydrogen
+        StartActionName = Start Liquefy Hydrogen
+        StopActionName = Stop Liquefy Hydrogen
+        AutoShutdown = false
+        GeneratesHeat = true
+        UseSpecialistBonus = false
+        INPUT_RESOURCE
+        {
+            ResourceName = Hydrogen
+            Ratio = 1
+        }
+        OUTPUT_RESOURCE
+        {
+            ResourceName = lqdHydrogen
+            Ratio = 0.00253785653674714
+            DumpExcess = false
+        }
+    }</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G17" s="2" t="e">
+      <c r="A17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2" t="n">
         <f aca="false">VLOOKUP(H17,Resources!$A$2:$F$799,5,0)/I17</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J17" s="2" t="e">
+        <v>0.0451529563736715</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2" t="n">
         <f aca="false">VLOOKUP(H17,Resources!$A$2:$F$799,4,0)*I17*G17</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K17" s="2" t="e">
+        <v>7.69E-007</v>
+      </c>
+      <c r="K17" s="2" t="n">
         <f aca="false">J17/VLOOKUP(H17,Resources!$A$2:$F$799,2,0)</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="N17" s="2" t="e">
         <f aca="false">VLOOKUP(L17,Resources!$A$2:$F$799,4,0)*M17*$G17</f>
@@ -2861,13 +2986,19 @@
         <f aca="false">R17/VLOOKUP(P17,Resources!$A$2:$F$799,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="V17" s="2" t="e">
+      <c r="T17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V17" s="2" t="n">
         <f aca="false">VLOOKUP(T17,Resources!$A$2:$F$799,4,0)*U17*$G17*$F17</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W17" s="2" t="e">
+        <v>7.68978326580941E-007</v>
+      </c>
+      <c r="W17" s="2" t="n">
         <f aca="false">V17/VLOOKUP(T17,Resources!$A$2:$F$799,2,0)</f>
-        <v>#N/A</v>
+        <v>0.00109525470243689</v>
       </c>
       <c r="Z17" s="2" t="e">
         <f aca="false">VLOOKUP(X17,Resources!$A$2:$F$799,4,0)*Y17*$G17*$F17</f>
@@ -2893,23 +3024,58 @@
         <f aca="false">AH17/VLOOKUP(AF17,Resources!$A$2:$F$799,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="AJ17" s="3" t="str">
+      <c r="AJ17" s="8" t="str">
         <f aca="false">Config!A17</f>
-        <v/>
+        <v>    MODULE
+    {
+        name = ModuleResourceConverter
+        ConverterName = Liquefy Ammonia
+        StartActionName = Start Liquefy Ammonia
+        StopActionName = Stop Liquefy Ammonia
+        AutoShutdown = false
+        GeneratesHeat = true
+        UseSpecialistBonus = false
+        INPUT_RESOURCE
+        {
+            ResourceName = Ammonia
+            Ratio = 1
+        }
+        OUTPUT_RESOURCE
+        {
+            ResourceName = lqdAmmonia
+            Ratio = 0.00109525470243689
+            DumpExcess = false
+        }
+    }</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G18" s="2" t="e">
+      <c r="A18" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2" t="n">
         <f aca="false">VLOOKUP(H18,Resources!$A$2:$F$799,5,0)/I18</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J18" s="2" t="e">
+        <v>0.0447007481296758</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2" t="n">
         <f aca="false">VLOOKUP(H18,Resources!$A$2:$F$799,4,0)*I18*G18</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K18" s="2" t="e">
+        <v>7.17E-007</v>
+      </c>
+      <c r="K18" s="2" t="n">
         <f aca="false">J18/VLOOKUP(H18,Resources!$A$2:$F$799,2,0)</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="N18" s="2" t="e">
         <f aca="false">VLOOKUP(L18,Resources!$A$2:$F$799,4,0)*M18*$G18</f>
@@ -2927,13 +3093,19 @@
         <f aca="false">R18/VLOOKUP(P18,Resources!$A$2:$F$799,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="V18" s="2" t="e">
+      <c r="T18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V18" s="2" t="n">
         <f aca="false">VLOOKUP(T18,Resources!$A$2:$F$799,4,0)*U18*$G18*$F18</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W18" s="2" t="e">
+        <v>7.17109963840399E-007</v>
+      </c>
+      <c r="W18" s="2" t="n">
         <f aca="false">V18/VLOOKUP(T18,Resources!$A$2:$F$799,2,0)</f>
-        <v>#N/A</v>
+        <v>0.00168489923601513</v>
       </c>
       <c r="Z18" s="2" t="e">
         <f aca="false">VLOOKUP(X18,Resources!$A$2:$F$799,4,0)*Y18*$G18*$F18</f>
@@ -2959,9 +3131,29 @@
         <f aca="false">AH18/VLOOKUP(AF18,Resources!$A$2:$F$799,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="AJ18" s="3" t="str">
+      <c r="AJ18" s="8" t="str">
         <f aca="false">Config!A18</f>
-        <v/>
+        <v>    MODULE
+    {
+        name = ModuleResourceConverter
+        ConverterName = Liquefy Methane
+        StartActionName = Start Liquefy Methane
+        StopActionName = Stop Liquefy Methane
+        AutoShutdown = false
+        GeneratesHeat = true
+        UseSpecialistBonus = false
+        INPUT_RESOURCE
+        {
+            ResourceName = Methane
+            Ratio = 1
+        }
+        OUTPUT_RESOURCE
+        {
+            ResourceName = lqdMethane
+            Ratio = 0.00168489923601513
+            DumpExcess = false
+        }
+    }</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5111,27 +5303,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B2" s="10" t="n">
         <v>0.01097</v>
@@ -5148,7 +5340,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B3" s="10" t="n">
         <v>0.0009</v>
@@ -5168,7 +5360,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B4" s="10" t="n">
         <v>0.001499</v>
@@ -5185,7 +5377,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B5" s="10" t="n">
         <v>0.001494</v>
@@ -5202,7 +5394,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B6" s="10" t="n">
         <v>0.00398</v>
@@ -5216,12 +5408,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B7" s="10" t="n">
         <v>0.0027</v>
@@ -5235,7 +5427,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5257,12 +5449,12 @@
         <v>0.0451529563736715</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B9" s="10" t="n">
         <v>0.00102</v>
@@ -5276,12 +5468,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B10" s="10" t="n">
         <v>7.085E-005</v>
@@ -5298,7 +5490,7 @@
     </row>
     <row r="11" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B11" s="10" t="n">
         <v>1.784E-006</v>
@@ -5312,12 +5504,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B12" s="10" t="n">
         <v>0.000719</v>
@@ -5334,7 +5526,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B13" s="10" t="n">
         <v>0.00246</v>
@@ -5348,7 +5540,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5370,7 +5562,7 @@
         <v>174.844097346533</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5392,7 +5584,7 @@
         <v>0.0443308339013861</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5414,12 +5606,12 @@
         <v>0.0446269189575152</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B17" s="10" t="n">
         <v>0.001501</v>
@@ -5436,7 +5628,7 @@
     </row>
     <row r="18" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B18" s="10" t="n">
         <v>0</v>
@@ -5453,7 +5645,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B19" s="10" t="n">
         <v>0.0025</v>
@@ -5470,7 +5662,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B20" s="10" t="n">
         <v>0.00177</v>
@@ -5484,12 +5676,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B21" s="10" t="n">
         <v>0.0019</v>
@@ -5503,12 +5695,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B22" s="10" t="n">
         <v>0.01097</v>
@@ -5525,7 +5717,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B23" s="10" t="n">
         <v>0.01097</v>
@@ -5542,7 +5734,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B24" s="10" t="n">
         <v>0.000421</v>
@@ -5556,12 +5748,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B25" s="10" t="n">
         <v>0.01097</v>
@@ -5578,7 +5770,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B26" s="10" t="n">
         <v>0.000544</v>
@@ -5592,12 +5784,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B27" s="10" t="n">
         <v>0.000789</v>
@@ -5617,7 +5809,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B28" s="10" t="n">
         <v>0.000568</v>
@@ -5631,12 +5823,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B29" s="10" t="n">
         <v>0</v>
@@ -5653,7 +5845,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B30" s="10" t="n">
         <v>0.0012517</v>
@@ -5670,7 +5862,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B31" s="10" t="n">
         <v>0.0013993</v>
@@ -5687,7 +5879,7 @@
     </row>
     <row r="32" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B32" s="10" t="n">
         <v>0.0014657</v>
@@ -5704,7 +5896,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B33" s="10" t="n">
         <v>1.696E-006</v>
@@ -5718,12 +5910,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B34" s="10" t="n">
         <v>0.001</v>
@@ -5740,7 +5932,7 @@
     </row>
     <row r="35" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B35" s="10" t="n">
         <v>0.00113</v>
@@ -5754,12 +5946,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B36" s="10" t="n">
         <v>1.786E-007</v>
@@ -5773,12 +5965,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B37" s="10" t="n">
         <v>0.002044</v>
@@ -5812,12 +6004,12 @@
         <v>42.0700709223194</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B39" s="10" t="n">
         <v>0.00177</v>
@@ -5834,7 +6026,7 @@
     </row>
     <row r="40" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B40" s="10" t="n">
         <v>0.0015</v>
@@ -5868,7 +6060,7 @@
         <v>31.3307844304725</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5890,12 +6082,12 @@
         <v>0.0891953566822106</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B43" s="10" t="n">
         <v>0.00086</v>
@@ -5915,7 +6107,7 @@
     </row>
     <row r="44" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B44" s="10" t="n">
         <v>0.005</v>
@@ -5932,7 +6124,7 @@
     </row>
     <row r="45" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B45" s="10" t="n">
         <v>0</v>
@@ -5949,7 +6141,7 @@
     </row>
     <row r="46" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B46" s="10" t="n">
         <v>0.001658</v>
@@ -5969,7 +6161,7 @@
     </row>
     <row r="47" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B47" s="10" t="n">
         <v>0.001995</v>
@@ -5986,7 +6178,7 @@
     </row>
     <row r="48" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B48" s="10" t="n">
         <v>0.001513</v>
@@ -6003,7 +6195,7 @@
     </row>
     <row r="49" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B49" s="10" t="n">
         <v>0.0025</v>
@@ -6023,7 +6215,7 @@
     </row>
     <row r="50" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B50" s="10" t="n">
         <v>0.0058</v>
@@ -6057,12 +6249,12 @@
         <v>4.81404743738862</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B52" s="10" t="n">
         <v>3.749E-006</v>
@@ -6079,7 +6271,7 @@
     </row>
     <row r="53" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="10" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B53" s="10" t="n">
         <v>0.01134</v>
@@ -6096,7 +6288,7 @@
     </row>
     <row r="54" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="10" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B54" s="10" t="n">
         <v>0.005</v>
@@ -6113,7 +6305,7 @@
     </row>
     <row r="55" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B55" s="10" t="n">
         <v>0.000534</v>
@@ -6127,12 +6319,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B56" s="10" t="n">
         <v>0.0007021</v>
@@ -6149,12 +6341,12 @@
         <v>41.225987227636</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="10" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B57" s="10" t="n">
         <v>0.00117325</v>
@@ -6168,12 +6360,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="10" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B58" s="10" t="n">
         <v>8.6E-005</v>
@@ -6190,7 +6382,7 @@
     </row>
     <row r="59" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="10" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B59" s="10" t="n">
         <v>0.001505</v>
@@ -6204,12 +6396,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="10" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B60" s="10" t="n">
         <v>0.0001786</v>
@@ -6226,7 +6418,7 @@
     </row>
     <row r="61" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B61" s="10" t="n">
         <v>0.0001786</v>
@@ -6243,7 +6435,7 @@
     </row>
     <row r="62" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="10" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B62" s="10" t="n">
         <v>7.085E-005</v>
@@ -6260,12 +6452,12 @@
         <v>35.1459412266603</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="10" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B63" s="10" t="n">
         <v>0.00042561</v>
@@ -6282,12 +6474,12 @@
         <v>26.5302204275404</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="10" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B64" s="10" t="n">
         <v>0.000824907</v>
@@ -6301,12 +6493,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="10" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B65" s="10" t="n">
         <v>0.001141</v>
@@ -6323,12 +6515,12 @@
         <v>35.6575871595185</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="10" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B66" s="10" t="n">
         <v>0.000133</v>
@@ -6345,7 +6537,7 @@
     </row>
     <row r="67" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="10" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B67" s="10" t="n">
         <v>0</v>
@@ -6362,7 +6554,7 @@
     </row>
     <row r="68" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="10" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B68" s="10" t="n">
         <v>0.0078</v>
@@ -6396,12 +6588,12 @@
         <v>0.0447007481296758</v>
       </c>
       <c r="F69" s="11" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="10" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B70" s="10" t="n">
         <v>0.0007918</v>
@@ -6415,12 +6607,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="10" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B71" s="10" t="n">
         <v>0.0027</v>
@@ -6437,7 +6629,7 @@
     </row>
     <row r="72" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="10" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B72" s="10" t="n">
         <v>0.00088</v>
@@ -6454,12 +6646,12 @@
         <v>19.1006460793536</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="10" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B73" s="10" t="n">
         <v>0.001429</v>
@@ -6479,7 +6671,7 @@
     </row>
     <row r="74" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="10" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B74" s="10" t="n">
         <v>0.001423</v>
@@ -6499,7 +6691,7 @@
     </row>
     <row r="75" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="10" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B75" s="10" t="n">
         <v>0.001407</v>
@@ -6519,7 +6711,7 @@
     </row>
     <row r="76" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="10" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B76" s="10" t="n">
         <v>0.001397</v>
@@ -6539,7 +6731,7 @@
     </row>
     <row r="77" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="10" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B77" s="10" t="n">
         <v>0.00138</v>
@@ -6559,7 +6751,7 @@
     </row>
     <row r="78" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="10" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B78" s="10" t="n">
         <v>0.001604</v>
@@ -6573,12 +6765,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="10" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B79" s="10" t="n">
         <v>9.002E-007</v>
@@ -6592,12 +6784,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="10" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B80" s="10" t="n">
         <v>0.0016</v>
@@ -6631,12 +6823,12 @@
         <v>0.0446571997686821</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="10" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="B82" s="10" t="n">
         <v>1.96E-006</v>
@@ -6653,7 +6845,7 @@
         <v>0.0653200515895101</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6675,12 +6867,12 @@
         <v>15.7589853387095</v>
       </c>
       <c r="F83" s="11" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="10" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B84" s="10" t="n">
         <v>0.0019</v>
@@ -6694,12 +6886,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="10" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B85" s="10" t="n">
         <v>0.0055</v>
@@ -6716,7 +6908,7 @@
     </row>
     <row r="86" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="10" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B86" s="10" t="n">
         <v>0.0036</v>
@@ -6733,7 +6925,7 @@
     </row>
     <row r="87" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="10" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B87" s="10" t="n">
         <v>0.005</v>
@@ -6767,12 +6959,12 @@
         <v>0.0881305081567598</v>
       </c>
       <c r="F88" s="11" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="10" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B89" s="10" t="n">
         <v>0.001772</v>
@@ -6789,7 +6981,7 @@
     </row>
     <row r="90" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="10" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B90" s="10" t="n">
         <v>0.000618</v>
@@ -6803,12 +6995,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F90" s="11" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="10" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B91" s="10" t="n">
         <v>0.019816</v>
@@ -6825,7 +7017,7 @@
     </row>
     <row r="92" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B92" s="10" t="n">
         <v>0.00104</v>
@@ -6842,7 +7034,7 @@
     </row>
     <row r="93" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="10" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B93" s="10" t="n">
         <v>0.00174</v>
@@ -6859,7 +7051,7 @@
     </row>
     <row r="94" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="10" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B94" s="10" t="n">
         <v>5E-005</v>
@@ -6876,7 +7068,7 @@
     </row>
     <row r="95" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="10" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B95" s="10" t="n">
         <v>0.0005</v>
@@ -6893,7 +7085,7 @@
     </row>
     <row r="96" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="10" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B96" s="10" t="n">
         <v>0.00378</v>
@@ -6910,7 +7102,7 @@
     </row>
     <row r="97" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="10" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B97" s="10" t="n">
         <v>0</v>
@@ -6927,7 +7119,7 @@
     </row>
     <row r="98" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="10" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B98" s="10" t="n">
         <v>0.0016</v>
@@ -6944,7 +7136,7 @@
     </row>
     <row r="99" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="10" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B99" s="10" t="n">
         <v>0.000851</v>
@@ -6961,12 +7153,12 @@
         <v>6.24660327184014</v>
       </c>
       <c r="F99" s="11" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="10" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="B100" s="10" t="n">
         <v>0</v>
@@ -6983,7 +7175,7 @@
     </row>
     <row r="101" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="10" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B101" s="10" t="n">
         <v>0.00070031</v>
@@ -7000,7 +7192,7 @@
     </row>
     <row r="102" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B102" s="10" t="n">
         <v>0.0022</v>
@@ -7017,7 +7209,7 @@
     </row>
     <row r="103" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="10" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="B103" s="10" t="n">
         <v>0</v>
@@ -7034,7 +7226,7 @@
     </row>
     <row r="104" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="10" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B104" s="10" t="n">
         <v>0.011724</v>
@@ -7051,7 +7243,7 @@
     </row>
     <row r="105" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="10" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B105" s="10" t="n">
         <v>0.000873</v>
@@ -7068,7 +7260,7 @@
     </row>
     <row r="106" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="10" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B106" s="10" t="n">
         <v>0.000811</v>
@@ -7085,7 +7277,7 @@
     </row>
     <row r="107" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="10" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B107" s="10" t="n">
         <v>0.000791</v>
@@ -7102,12 +7294,12 @@
         <v>13.1617655867918</v>
       </c>
       <c r="F107" s="11" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="10" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B108" s="10" t="n">
         <v>0.000829</v>
@@ -7124,7 +7316,7 @@
     </row>
     <row r="109" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="10" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B109" s="10" t="n">
         <v>0.0075</v>
@@ -7141,7 +7333,7 @@
     </row>
     <row r="110" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="10" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B110" s="10" t="n">
         <v>0.0113</v>
@@ -7158,7 +7350,7 @@
     </row>
     <row r="111" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="10" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B111" s="10" t="n">
         <v>0</v>
@@ -7175,7 +7367,7 @@
     </row>
     <row r="112" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="10" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B112" s="10" t="n">
         <v>0.00075</v>
@@ -7192,7 +7384,7 @@
     </row>
     <row r="113" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B113" s="10" t="n">
         <v>0</v>
@@ -7209,7 +7401,7 @@
     </row>
     <row r="114" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="10" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B114" s="10" t="n">
         <v>0.001005</v>
@@ -7243,12 +7435,12 @@
         <v>55.508435061792</v>
       </c>
       <c r="F115" s="11" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="10" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B116" s="10" t="n">
         <v>0.0001</v>
@@ -7265,7 +7457,7 @@
         <v>0.761655229143976</v>
       </c>
       <c r="F116" s="11" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -7297,7 +7489,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -8571,17 +8763,42 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="str">
+      <c r="A15" s="15" t="str">
         <f aca="false">IF(ISBLANK(Conversion!A15),"",CONCATENATE("    MODULE", CHAR(10), "    {", CHAR(10), "        name = ModuleResourceConverter", CHAR(10), "        ConverterName = ", Conversion!A15, CHAR(10), "        StartActionName = Start ", Conversion!A15, CHAR(10), "        StopActionName = Stop ", Conversion!A15, CHAR(10), "        AutoShutdown = false", CHAR(10), "        GeneratesHeat = true", CHAR(10), "        UseSpecialistBonus = false", CHAR(10), B15, C15, D15, E15, F15, G15, H15, I15, J15, CHAR(10), "    }"))</f>
-        <v/>
+        <v>    MODULE
+    {
+        name = ModuleResourceConverter
+        ConverterName = Liquefy Oxygen
+        StartActionName = Start Liquefy Oxygen
+        StopActionName = Stop Liquefy Oxygen
+        AutoShutdown = false
+        GeneratesHeat = true
+        UseSpecialistBonus = false
+        INPUT_RESOURCE
+        {
+            ResourceName = Oxygen
+            Ratio = 1
+        }
+        OUTPUT_RESOURCE
+        {
+            ResourceName = lqdOxygen
+            Ratio = 0.00247157800561483
+            DumpExcess = false
+        }
+    }</v>
       </c>
       <c r="B15" s="0" t="str">
         <f aca="false">IF(ISBLANK(Conversion!B15),"",CONCATENATE(CHAR(10),"        INPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ElectricCharge", CHAR(10), "            Ratio = ", Conversion!B15, CHAR(10), "        }"))</f>
         <v/>
       </c>
-      <c r="C15" s="0" t="str">
+      <c r="C15" s="15" t="str">
         <f aca="false">IF(ISBLANK(Conversion!I15),"",CONCATENATE(CHAR(10),"        INPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ", Conversion!H15, CHAR(10), "            Ratio = ", Conversion!K15, CHAR(10), "        }"))</f>
-        <v/>
+        <v>
+        INPUT_RESOURCE
+        {
+            ResourceName = Oxygen
+            Ratio = 1
+        }</v>
       </c>
       <c r="D15" s="0" t="str">
         <f aca="false">IF(ISBLANK(Conversion!M15),"",CONCATENATE(CHAR(10),"        INPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ", Conversion!L15, CHAR(10), "            Ratio = ", Conversion!O15, CHAR(10), "        }"))</f>
@@ -8595,9 +8812,15 @@
         <f aca="false">IF(ISBLANK(Conversion!C15),"",CONCATENATE(CHAR(10), "        OUTPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ElectricCharge", CHAR(10), "            Ratio = ", Conversion!C15, CHAR(10), "            DumpExcess = true", CHAR(10), "        }"))</f>
         <v/>
       </c>
-      <c r="G15" s="0" t="str">
+      <c r="G15" s="15" t="str">
         <f aca="false">IF(ISBLANK(Conversion!U15),"",CONCATENATE(CHAR(10), "        OUTPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ", Conversion!T15, CHAR(10), "            Ratio = ", Conversion!W15, CHAR(10), "            DumpExcess = false", CHAR(10), "        }"))</f>
-        <v/>
+        <v>
+        OUTPUT_RESOURCE
+        {
+            ResourceName = lqdOxygen
+            Ratio = 0.00247157800561483
+            DumpExcess = false
+        }</v>
       </c>
       <c r="H15" s="0" t="str">
         <f aca="false">IF(ISBLANK(Conversion!Y15),"",CONCATENATE(CHAR(10), "        OUTPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ", Conversion!X15, CHAR(10), "            Ratio = ", Conversion!AA15, CHAR(10), "            DumpExcess = false", CHAR(10), "        }"))</f>
@@ -8613,17 +8836,42 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="str">
+      <c r="A16" s="15" t="str">
         <f aca="false">IF(ISBLANK(Conversion!A16),"",CONCATENATE("    MODULE", CHAR(10), "    {", CHAR(10), "        name = ModuleResourceConverter", CHAR(10), "        ConverterName = ", Conversion!A16, CHAR(10), "        StartActionName = Start ", Conversion!A16, CHAR(10), "        StopActionName = Stop ", Conversion!A16, CHAR(10), "        AutoShutdown = false", CHAR(10), "        GeneratesHeat = true", CHAR(10), "        UseSpecialistBonus = false", CHAR(10), B16, C16, D16, E16, F16, G16, H16, I16, J16, CHAR(10), "    }"))</f>
-        <v/>
+        <v>    MODULE
+    {
+        name = ModuleResourceConverter
+        ConverterName = Liquefy Hydrogen
+        StartActionName = Start Liquefy Hydrogen
+        StopActionName = Stop Liquefy Hydrogen
+        AutoShutdown = false
+        GeneratesHeat = true
+        UseSpecialistBonus = false
+        INPUT_RESOURCE
+        {
+            ResourceName = Hydrogen
+            Ratio = 1
+        }
+        OUTPUT_RESOURCE
+        {
+            ResourceName = lqdHydrogen
+            Ratio = 0.00253785653674714
+            DumpExcess = false
+        }
+    }</v>
       </c>
       <c r="B16" s="0" t="str">
         <f aca="false">IF(ISBLANK(Conversion!B16),"",CONCATENATE(CHAR(10),"        INPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ElectricCharge", CHAR(10), "            Ratio = ", Conversion!B16, CHAR(10), "        }"))</f>
         <v/>
       </c>
-      <c r="C16" s="0" t="str">
+      <c r="C16" s="15" t="str">
         <f aca="false">IF(ISBLANK(Conversion!I16),"",CONCATENATE(CHAR(10),"        INPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ", Conversion!H16, CHAR(10), "            Ratio = ", Conversion!K16, CHAR(10), "        }"))</f>
-        <v/>
+        <v>
+        INPUT_RESOURCE
+        {
+            ResourceName = Hydrogen
+            Ratio = 1
+        }</v>
       </c>
       <c r="D16" s="0" t="str">
         <f aca="false">IF(ISBLANK(Conversion!M16),"",CONCATENATE(CHAR(10),"        INPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ", Conversion!L16, CHAR(10), "            Ratio = ", Conversion!O16, CHAR(10), "        }"))</f>
@@ -8637,9 +8885,15 @@
         <f aca="false">IF(ISBLANK(Conversion!C16),"",CONCATENATE(CHAR(10), "        OUTPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ElectricCharge", CHAR(10), "            Ratio = ", Conversion!C16, CHAR(10), "            DumpExcess = true", CHAR(10), "        }"))</f>
         <v/>
       </c>
-      <c r="G16" s="0" t="str">
+      <c r="G16" s="15" t="str">
         <f aca="false">IF(ISBLANK(Conversion!U16),"",CONCATENATE(CHAR(10), "        OUTPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ", Conversion!T16, CHAR(10), "            Ratio = ", Conversion!W16, CHAR(10), "            DumpExcess = false", CHAR(10), "        }"))</f>
-        <v/>
+        <v>
+        OUTPUT_RESOURCE
+        {
+            ResourceName = lqdHydrogen
+            Ratio = 0.00253785653674714
+            DumpExcess = false
+        }</v>
       </c>
       <c r="H16" s="0" t="str">
         <f aca="false">IF(ISBLANK(Conversion!Y16),"",CONCATENATE(CHAR(10), "        OUTPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ", Conversion!X16, CHAR(10), "            Ratio = ", Conversion!AA16, CHAR(10), "            DumpExcess = false", CHAR(10), "        }"))</f>
@@ -8655,17 +8909,42 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="str">
+      <c r="A17" s="15" t="str">
         <f aca="false">IF(ISBLANK(Conversion!A17),"",CONCATENATE("    MODULE", CHAR(10), "    {", CHAR(10), "        name = ModuleResourceConverter", CHAR(10), "        ConverterName = ", Conversion!A17, CHAR(10), "        StartActionName = Start ", Conversion!A17, CHAR(10), "        StopActionName = Stop ", Conversion!A17, CHAR(10), "        AutoShutdown = false", CHAR(10), "        GeneratesHeat = true", CHAR(10), "        UseSpecialistBonus = false", CHAR(10), B17, C17, D17, E17, F17, G17, H17, I17, J17, CHAR(10), "    }"))</f>
-        <v/>
+        <v>    MODULE
+    {
+        name = ModuleResourceConverter
+        ConverterName = Liquefy Ammonia
+        StartActionName = Start Liquefy Ammonia
+        StopActionName = Stop Liquefy Ammonia
+        AutoShutdown = false
+        GeneratesHeat = true
+        UseSpecialistBonus = false
+        INPUT_RESOURCE
+        {
+            ResourceName = Ammonia
+            Ratio = 1
+        }
+        OUTPUT_RESOURCE
+        {
+            ResourceName = lqdAmmonia
+            Ratio = 0.00109525470243689
+            DumpExcess = false
+        }
+    }</v>
       </c>
       <c r="B17" s="0" t="str">
         <f aca="false">IF(ISBLANK(Conversion!B17),"",CONCATENATE(CHAR(10),"        INPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ElectricCharge", CHAR(10), "            Ratio = ", Conversion!B17, CHAR(10), "        }"))</f>
         <v/>
       </c>
-      <c r="C17" s="0" t="str">
+      <c r="C17" s="15" t="str">
         <f aca="false">IF(ISBLANK(Conversion!I17),"",CONCATENATE(CHAR(10),"        INPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ", Conversion!H17, CHAR(10), "            Ratio = ", Conversion!K17, CHAR(10), "        }"))</f>
-        <v/>
+        <v>
+        INPUT_RESOURCE
+        {
+            ResourceName = Ammonia
+            Ratio = 1
+        }</v>
       </c>
       <c r="D17" s="0" t="str">
         <f aca="false">IF(ISBLANK(Conversion!M17),"",CONCATENATE(CHAR(10),"        INPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ", Conversion!L17, CHAR(10), "            Ratio = ", Conversion!O17, CHAR(10), "        }"))</f>
@@ -8679,9 +8958,15 @@
         <f aca="false">IF(ISBLANK(Conversion!C17),"",CONCATENATE(CHAR(10), "        OUTPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ElectricCharge", CHAR(10), "            Ratio = ", Conversion!C17, CHAR(10), "            DumpExcess = true", CHAR(10), "        }"))</f>
         <v/>
       </c>
-      <c r="G17" s="0" t="str">
+      <c r="G17" s="15" t="str">
         <f aca="false">IF(ISBLANK(Conversion!U17),"",CONCATENATE(CHAR(10), "        OUTPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ", Conversion!T17, CHAR(10), "            Ratio = ", Conversion!W17, CHAR(10), "            DumpExcess = false", CHAR(10), "        }"))</f>
-        <v/>
+        <v>
+        OUTPUT_RESOURCE
+        {
+            ResourceName = lqdAmmonia
+            Ratio = 0.00109525470243689
+            DumpExcess = false
+        }</v>
       </c>
       <c r="H17" s="0" t="str">
         <f aca="false">IF(ISBLANK(Conversion!Y17),"",CONCATENATE(CHAR(10), "        OUTPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ", Conversion!X17, CHAR(10), "            Ratio = ", Conversion!AA17, CHAR(10), "            DumpExcess = false", CHAR(10), "        }"))</f>
@@ -8697,17 +8982,42 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="str">
+      <c r="A18" s="15" t="str">
         <f aca="false">IF(ISBLANK(Conversion!A18),"",CONCATENATE("    MODULE", CHAR(10), "    {", CHAR(10), "        name = ModuleResourceConverter", CHAR(10), "        ConverterName = ", Conversion!A18, CHAR(10), "        StartActionName = Start ", Conversion!A18, CHAR(10), "        StopActionName = Stop ", Conversion!A18, CHAR(10), "        AutoShutdown = false", CHAR(10), "        GeneratesHeat = true", CHAR(10), "        UseSpecialistBonus = false", CHAR(10), B18, C18, D18, E18, F18, G18, H18, I18, J18, CHAR(10), "    }"))</f>
-        <v/>
+        <v>    MODULE
+    {
+        name = ModuleResourceConverter
+        ConverterName = Liquefy Methane
+        StartActionName = Start Liquefy Methane
+        StopActionName = Stop Liquefy Methane
+        AutoShutdown = false
+        GeneratesHeat = true
+        UseSpecialistBonus = false
+        INPUT_RESOURCE
+        {
+            ResourceName = Methane
+            Ratio = 1
+        }
+        OUTPUT_RESOURCE
+        {
+            ResourceName = lqdMethane
+            Ratio = 0.00168489923601513
+            DumpExcess = false
+        }
+    }</v>
       </c>
       <c r="B18" s="0" t="str">
         <f aca="false">IF(ISBLANK(Conversion!B18),"",CONCATENATE(CHAR(10),"        INPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ElectricCharge", CHAR(10), "            Ratio = ", Conversion!B18, CHAR(10), "        }"))</f>
         <v/>
       </c>
-      <c r="C18" s="0" t="str">
+      <c r="C18" s="15" t="str">
         <f aca="false">IF(ISBLANK(Conversion!I18),"",CONCATENATE(CHAR(10),"        INPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ", Conversion!H18, CHAR(10), "            Ratio = ", Conversion!K18, CHAR(10), "        }"))</f>
-        <v/>
+        <v>
+        INPUT_RESOURCE
+        {
+            ResourceName = Methane
+            Ratio = 1
+        }</v>
       </c>
       <c r="D18" s="0" t="str">
         <f aca="false">IF(ISBLANK(Conversion!M18),"",CONCATENATE(CHAR(10),"        INPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ", Conversion!L18, CHAR(10), "            Ratio = ", Conversion!O18, CHAR(10), "        }"))</f>
@@ -8721,9 +9031,15 @@
         <f aca="false">IF(ISBLANK(Conversion!C18),"",CONCATENATE(CHAR(10), "        OUTPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ElectricCharge", CHAR(10), "            Ratio = ", Conversion!C18, CHAR(10), "            DumpExcess = true", CHAR(10), "        }"))</f>
         <v/>
       </c>
-      <c r="G18" s="0" t="str">
+      <c r="G18" s="15" t="str">
         <f aca="false">IF(ISBLANK(Conversion!U18),"",CONCATENATE(CHAR(10), "        OUTPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ", Conversion!T18, CHAR(10), "            Ratio = ", Conversion!W18, CHAR(10), "            DumpExcess = false", CHAR(10), "        }"))</f>
-        <v/>
+        <v>
+        OUTPUT_RESOURCE
+        {
+            ResourceName = lqdMethane
+            Ratio = 0.00168489923601513
+            DumpExcess = false
+        }</v>
       </c>
       <c r="H18" s="0" t="str">
         <f aca="false">IF(ISBLANK(Conversion!Y18),"",CONCATENATE(CHAR(10), "        OUTPUT_RESOURCE", CHAR(10), "        {", CHAR(10), "            ResourceName = ", Conversion!X18, CHAR(10), "            Ratio = ", Conversion!AA18, CHAR(10), "            DumpExcess = false", CHAR(10), "        }"))</f>
@@ -10963,25 +11279,25 @@
         <v>13</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>16</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="I1" s="19" t="s">
         <v>17</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11518,20 +11834,20 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16" t="n">
+      <c r="A15" s="16" t="str">
         <f aca="false">Conversion!A15</f>
-        <v>0</v>
+        <v>Liquefy Oxygen</v>
       </c>
       <c r="B15" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="16" t="n">
+      <c r="C15" s="16" t="str">
         <f aca="false">Conversion!T15</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="16" t="e">
+        <v>lqdOxygen</v>
+      </c>
+      <c r="D15" s="16" t="n">
         <f aca="false">Conversion!W15*B15</f>
-        <v>#N/A</v>
+        <v>0.00247157800561483</v>
       </c>
       <c r="E15" s="16" t="n">
         <f aca="false">Conversion!X15</f>
@@ -11559,20 +11875,20 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="n">
+      <c r="A16" s="16" t="str">
         <f aca="false">Conversion!A16</f>
-        <v>0</v>
+        <v>Liquefy Hydrogen</v>
       </c>
       <c r="B16" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="C16" s="16" t="n">
+      <c r="C16" s="16" t="str">
         <f aca="false">Conversion!T16</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="16" t="e">
+        <v>lqdHydrogen</v>
+      </c>
+      <c r="D16" s="16" t="n">
         <f aca="false">Conversion!W16*B16</f>
-        <v>#N/A</v>
+        <v>0.00253785653674714</v>
       </c>
       <c r="E16" s="16" t="n">
         <f aca="false">Conversion!X16</f>
@@ -11600,20 +11916,20 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16" t="n">
+      <c r="A17" s="16" t="str">
         <f aca="false">Conversion!A17</f>
-        <v>0</v>
+        <v>Liquefy Ammonia</v>
       </c>
       <c r="B17" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="C17" s="16" t="n">
+      <c r="C17" s="16" t="str">
         <f aca="false">Conversion!T17</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="16" t="e">
+        <v>lqdAmmonia</v>
+      </c>
+      <c r="D17" s="16" t="n">
         <f aca="false">Conversion!W17*B17</f>
-        <v>#N/A</v>
+        <v>0.00109525470243689</v>
       </c>
       <c r="E17" s="16" t="n">
         <f aca="false">Conversion!X17</f>
@@ -11641,20 +11957,20 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="n">
+      <c r="A18" s="16" t="str">
         <f aca="false">Conversion!A18</f>
-        <v>0</v>
+        <v>Liquefy Methane</v>
       </c>
       <c r="B18" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="C18" s="16" t="n">
+      <c r="C18" s="16" t="str">
         <f aca="false">Conversion!T18</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="16" t="e">
+        <v>lqdMethane</v>
+      </c>
+      <c r="D18" s="16" t="n">
         <f aca="false">Conversion!W18*B18</f>
-        <v>#N/A</v>
+        <v>0.00168489923601513</v>
       </c>
       <c r="E18" s="16" t="n">
         <f aca="false">Conversion!X18</f>

</xml_diff>